<commit_message>
Some spreadsheet changes and better contours.
</commit_message>
<xml_diff>
--- a/ExperimentalData/Induced EMF/Induced Rectangular 2016-03-02 20x50.xlsx
+++ b/ExperimentalData/Induced EMF/Induced Rectangular 2016-03-02 20x50.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17460" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="20x50 5-5" sheetId="2" r:id="rId1"/>
     <sheet name="60x50 5-10" sheetId="3" r:id="rId2"/>
-    <sheet name="Template" sheetId="1" r:id="rId3"/>
+    <sheet name="40x50 5-10" sheetId="4" r:id="rId3"/>
+    <sheet name="Template" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -257,6 +258,117 @@
       <text>
         <r>
           <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>This is the peak to peak voltage changed as measured across the inline resistor of the driven circuit.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Left to right width of the circuit measured at the wire outer edge, hence the center to center width is this value munus one wire width.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B10" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Distance from the front to rear wires of the circuit measured at the wire outer edge, hence the center to center distance is this value munus one wire width.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K10" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Distance from driver front (Df) to passive front (Pf) in meters.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L10" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Distance from driver front (Df) to passive front (Pf) in meters.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="M10" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Distance from driver front (Df) to passive rear (Pr) in meters.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N10" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Distance from driver rear (Dr) to passive front (Pf) in meters.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O10" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+          </rPr>
+          <t>Distance from driver rear (Dr) to passive rear (Pr) in meters.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Microsoft Office User</author>
+  </authors>
+  <commentList>
+    <comment ref="G7" authorId="0">
+      <text>
+        <r>
+          <rPr>
             <sz val="10"/>
             <color indexed="81"/>
             <rFont val="Calibri"/>
@@ -344,7 +456,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="60">
   <si>
     <t>Date:</t>
   </si>
@@ -514,13 +626,16 @@
     <t>For 37.2mV EMF, -16.6mv to 20.6mV</t>
   </si>
   <si>
-    <t>Maxwell near (mv)</t>
+    <t>Repeat EMF x2 (mv)</t>
   </si>
   <si>
-    <t>Maxwell far (mv)</t>
+    <t>3:35pm</t>
   </si>
   <si>
-    <t>BAD DATA</t>
+    <t>5:21pm</t>
+  </si>
+  <si>
+    <t>-3.66V to 3.72V</t>
   </si>
 </sst>
 </file>
@@ -593,7 +708,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -614,6 +729,17 @@
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -646,7 +772,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -679,17 +805,21 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -761,31 +891,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.00182</c:v>
+                  <c:v>0.00175</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0036</c:v>
+                  <c:v>0.00254</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.00459</c:v>
+                  <c:v>0.00363</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.00553</c:v>
+                  <c:v>0.00463</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.00648</c:v>
+                  <c:v>0.00577</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0076</c:v>
+                  <c:v>0.00725</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.00829</c:v>
+                  <c:v>0.0084</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.00944</c:v>
+                  <c:v>0.00994</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.01025</c:v>
+                  <c:v>0.01274</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -797,31 +927,31 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>35.85</c:v>
+                  <c:v>47.2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>28.915</c:v>
+                  <c:v>39.9</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>26.9</c:v>
+                  <c:v>33.3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>24.75</c:v>
+                  <c:v>28.45</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>23.3</c:v>
+                  <c:v>24.95</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>22.45</c:v>
+                  <c:v>20.8</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>21.75</c:v>
+                  <c:v>18.55</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>20.75</c:v>
+                  <c:v>15.7</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>20.15</c:v>
+                  <c:v>12.55</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -865,31 +995,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.00182</c:v>
+                  <c:v>0.00175</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0036</c:v>
+                  <c:v>0.00254</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.00459</c:v>
+                  <c:v>0.00363</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.00553</c:v>
+                  <c:v>0.00463</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.00648</c:v>
+                  <c:v>0.00577</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0076</c:v>
+                  <c:v>0.00725</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.00829</c:v>
+                  <c:v>0.0084</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.00944</c:v>
+                  <c:v>0.00994</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.01025</c:v>
+                  <c:v>0.01274</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -901,31 +1031,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>104.265884148792</c:v>
+                  <c:v>351.0114648216787</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>48.54124107366092</c:v>
+                  <c:v>232.9650555690588</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>36.44923929143771</c:v>
+                  <c:v>155.0994796237268</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>29.06796502240024</c:v>
+                  <c:v>116.3741527895794</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>23.85419846062637</c:v>
+                  <c:v>88.98270763660982</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>19.4508007216983</c:v>
+                  <c:v>66.69387568195184</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>17.36123101761379</c:v>
+                  <c:v>55.04434387954952</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>14.59897975890512</c:v>
+                  <c:v>43.91321154558727</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>13.0517055925882</c:v>
+                  <c:v>31.04325814839811</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -969,31 +1099,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>0.00182</c:v>
+                  <c:v>0.00175</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0036</c:v>
+                  <c:v>0.00254</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.00459</c:v>
+                  <c:v>0.00363</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.00553</c:v>
+                  <c:v>0.00463</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.00648</c:v>
+                  <c:v>0.00577</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0076</c:v>
+                  <c:v>0.00725</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.00829</c:v>
+                  <c:v>0.0084</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.00944</c:v>
+                  <c:v>0.00994</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.01025</c:v>
+                  <c:v>0.01274</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1005,31 +1135,31 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="9"/>
                 <c:pt idx="0">
-                  <c:v>27.03529326364297</c:v>
+                  <c:v>98.75208366358103</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>19.90572771107074</c:v>
+                  <c:v>84.42983836688934</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17.53003409008075</c:v>
+                  <c:v>71.28407970927973</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>15.78314516534624</c:v>
+                  <c:v>62.74073954929306</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>14.35448566915121</c:v>
+                  <c:v>55.36053234602955</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>12.97661600842937</c:v>
+                  <c:v>48.10661792802854</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>12.25216288871262</c:v>
+                  <c:v>43.67029243833719</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>11.20625992315141</c:v>
+                  <c:v>38.84991788081766</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>10.56740931164482</c:v>
+                  <c:v>32.26997680590967</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1271,6 +1401,9 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>Measured</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -1384,6 +1517,9 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:v>1/x rule</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -1457,37 +1593,37 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>233.7477040713648</c:v>
+                  <c:v>259.302598234357</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>208.5117291654034</c:v>
+                  <c:v>231.307654334951</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>139.774094668856</c:v>
+                  <c:v>155.0551525521032</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>85.9446256076194</c:v>
+                  <c:v>95.34067858707525</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>63.48197142867239</c:v>
+                  <c:v>70.42225376240828</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>40.1796365967435</c:v>
+                  <c:v>44.5723486655807</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>34.42879551247182</c:v>
+                  <c:v>38.1927863887711</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>27.94351018531616</c:v>
+                  <c:v>30.99848541241073</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>19.09221456728826</c:v>
+                  <c:v>21.17950575392269</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>14.74038076010347</c:v>
+                  <c:v>16.35189977691335</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>6.640485001560448</c:v>
+                  <c:v>7.366468138293226</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1497,6 +1633,9 @@
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
+          <c:tx>
+            <c:v>Maxwells</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="19050" cap="rnd">
               <a:solidFill>
@@ -1570,37 +1709,123 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="11"/>
                 <c:pt idx="0">
-                  <c:v>119.3111878829002</c:v>
+                  <c:v>118.0236570784086</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>114.7400818576905</c:v>
+                  <c:v>113.5018795354852</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>99.20894053877637</c:v>
+                  <c:v>98.13834046101984</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>81.5501681455155</c:v>
+                  <c:v>80.67013035977256</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>71.38846867018711</c:v>
+                  <c:v>70.61808951187577</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>57.47957135780069</c:v>
+                  <c:v>56.85928821365178</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>53.2037740468328</c:v>
+                  <c:v>52.62963260028426</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>47.77853761265059</c:v>
+                  <c:v>47.26294188301769</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>38.9293157948917</c:v>
+                  <c:v>38.50921526473102</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>33.68247731956509</c:v>
+                  <c:v>33.31899734849065</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>21.0643663747123</c:v>
+                  <c:v>20.83705306851038</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:v>Maxwell Near</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'60x50 5-10'!$L$11:$L$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.00254</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.00283</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.00411</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.00638</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.00831</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.01218</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.01379</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.01624</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.02161</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.02599</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.04384</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'60x50 5-10'!#REF!</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1819,6 +2044,610 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'40x50 5-10'!$L$11:$L$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="17"/>
+                <c:pt idx="0">
+                  <c:v>0.00198</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.00271</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.00334</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.00405</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.00487</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0057</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.00715</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.00906</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.01052</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.01323</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.01553</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.01781</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.01965</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.02405</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.03022</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.03736</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'40x50 5-10'!$K$11:$K$26</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>105.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>91.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>82.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>74.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>67.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>52.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>43.75</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>38.85</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>31.9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>27.3</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>23.7</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>20.8</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>17.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>13.1</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>9.35</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'40x50 5-10'!$L$11:$L$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>0.00198</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.00271</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.00334</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.00405</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.00487</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0057</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.00715</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.00906</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.01052</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.01323</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.01553</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.01781</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.01965</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.02405</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.03022</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.03736</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'40x50 5-10'!$R$11:$R$26</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>118.5285503779612</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>105.4699569001612</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>96.93543117882129</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>89.20668143347089</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>81.9627674746404</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>75.913059061936</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>67.4498566320709</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>58.97476789416105</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>53.84697645376768</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>46.35645324456893</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>41.41666694909346</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>37.40664624581065</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>34.65562178559666</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>29.35245359646682</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>23.9538722381101</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>19.52619750088495</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Maxwell Near</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent4"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'40x50 5-10'!$L$11:$L$21</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>0.00198</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.00271</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.00334</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.00405</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.00487</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.0057</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.00715</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.00906</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.01052</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.01323</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.01553</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'60x50 5-10'!#REF!</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="-2013045136"/>
+        <c:axId val="-2012474576"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="-2013045136"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2012474576"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="-2012474576"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2013045136"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -1899,6 +2728,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -2416,6 +3285,522 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2980,6 +4365,43 @@
       <xdr:colOff>264160</xdr:colOff>
       <xdr:row>45</xdr:row>
       <xdr:rowOff>13546</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>1123769</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>91467</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>445589</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>194975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3271,8 +4693,8 @@
   </sheetPr>
   <dimension ref="B4:R31"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B6" zoomScale="98" workbookViewId="0">
-      <selection activeCell="S27" sqref="S27"/>
+    <sheetView showGridLines="0" topLeftCell="A7" zoomScale="98" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3297,26 +4719,24 @@
         <v>0</v>
       </c>
       <c r="C4" s="19">
-        <v>42431</v>
+        <v>42435</v>
       </c>
       <c r="D4" s="19"/>
       <c r="G4" s="1" t="s">
         <v>18</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="J4" s="20" t="s">
-        <v>58</v>
-      </c>
-      <c r="K4" s="20"/>
-      <c r="L4" s="20"/>
-      <c r="M4" s="20"/>
-      <c r="N4" s="20"/>
-      <c r="O4" s="20"/>
-      <c r="P4" s="20"/>
-      <c r="Q4" s="20"/>
-      <c r="R4" s="20"/>
+        <v>57</v>
+      </c>
+      <c r="J4" s="23"/>
+      <c r="K4" s="23"/>
+      <c r="L4" s="23"/>
+      <c r="M4" s="23"/>
+      <c r="N4" s="23"/>
+      <c r="O4" s="23"/>
+      <c r="P4" s="23"/>
+      <c r="Q4" s="23"/>
+      <c r="R4" s="23"/>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
@@ -3330,15 +4750,15 @@
       <c r="H5" s="5">
         <v>200000</v>
       </c>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="20"/>
-      <c r="M5" s="20"/>
-      <c r="N5" s="20"/>
-      <c r="O5" s="20"/>
-      <c r="P5" s="20"/>
-      <c r="Q5" s="20"/>
-      <c r="R5" s="20"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
+      <c r="L5" s="23"/>
+      <c r="M5" s="23"/>
+      <c r="N5" s="23"/>
+      <c r="O5" s="23"/>
+      <c r="P5" s="23"/>
+      <c r="Q5" s="23"/>
+      <c r="R5" s="23"/>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.2">
       <c r="G6" s="1" t="s">
@@ -3347,15 +4767,15 @@
       <c r="H6" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="J6" s="20"/>
-      <c r="K6" s="20"/>
-      <c r="L6" s="20"/>
-      <c r="M6" s="20"/>
-      <c r="N6" s="20"/>
-      <c r="O6" s="20"/>
-      <c r="P6" s="20"/>
-      <c r="Q6" s="20"/>
-      <c r="R6" s="20"/>
+      <c r="J6" s="23"/>
+      <c r="K6" s="23"/>
+      <c r="L6" s="23"/>
+      <c r="M6" s="23"/>
+      <c r="N6" s="23"/>
+      <c r="O6" s="23"/>
+      <c r="P6" s="23"/>
+      <c r="Q6" s="23"/>
+      <c r="R6" s="23"/>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B7" s="4"/>
@@ -3371,15 +4791,15 @@
       <c r="H7" s="3">
         <v>14.15</v>
       </c>
-      <c r="J7" s="20"/>
-      <c r="K7" s="20"/>
-      <c r="L7" s="20"/>
-      <c r="M7" s="20"/>
-      <c r="N7" s="20"/>
-      <c r="O7" s="20"/>
-      <c r="P7" s="20"/>
-      <c r="Q7" s="20"/>
-      <c r="R7" s="20"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="23"/>
+      <c r="L7" s="23"/>
+      <c r="M7" s="23"/>
+      <c r="N7" s="23"/>
+      <c r="O7" s="23"/>
+      <c r="P7" s="23"/>
+      <c r="Q7" s="23"/>
+      <c r="R7" s="23"/>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
@@ -3458,45 +4878,43 @@
         <v>5</v>
       </c>
       <c r="G11" s="3">
-        <v>12.19</v>
+        <v>12.07</v>
       </c>
       <c r="H11" s="5">
-        <v>71.7</v>
-      </c>
-      <c r="I11" s="5">
-        <v>1.9</v>
-      </c>
+        <v>94.4</v>
+      </c>
+      <c r="I11" s="5"/>
       <c r="K11" s="18">
         <f>H11/2</f>
-        <v>35.85</v>
+        <v>47.2</v>
       </c>
       <c r="L11" s="2">
         <f>0.001*(G11-$C$19+$C$20)</f>
-        <v>1.82E-3</v>
+        <v>1.75E-3</v>
       </c>
       <c r="M11" s="2">
         <f>L11+$D$25</f>
-        <v>2.214E-2</v>
+        <v>2.2070000000000003E-2</v>
       </c>
       <c r="N11" s="2">
         <f>L11+$C$25</f>
-        <v>8.2040000000000002E-2</v>
+        <v>8.1970000000000001E-2</v>
       </c>
       <c r="O11" s="2">
         <f>L11+$C$25+$D$25</f>
-        <v>0.10236000000000001</v>
+        <v>0.10229000000000001</v>
       </c>
       <c r="P11" s="12">
         <f>1/L11-1/M11-1/N11+1/O11</f>
-        <v>501.86369628896188</v>
+        <v>523.69473683694923</v>
       </c>
       <c r="Q11" s="12">
         <f>$C$28*$C$29*P11*1000</f>
-        <v>104.26588414879198</v>
+        <v>351.01146482167866</v>
       </c>
       <c r="R11" s="12">
         <f>$C$31*(LN(M11/L11)+LN(N11/O11))*1000</f>
-        <v>27.03529326364297</v>
+        <v>98.752083663581033</v>
       </c>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.2">
@@ -3510,45 +4928,43 @@
         <v>1.78</v>
       </c>
       <c r="G12" s="3">
-        <v>13.97</v>
+        <v>12.86</v>
       </c>
       <c r="H12" s="5">
-        <v>57.83</v>
-      </c>
-      <c r="I12" s="5">
-        <v>2.11</v>
-      </c>
+        <v>79.8</v>
+      </c>
+      <c r="I12" s="5"/>
       <c r="K12" s="18">
         <f t="shared" ref="K12:K19" si="0">H12/2</f>
-        <v>28.914999999999999</v>
+        <v>39.9</v>
       </c>
       <c r="L12" s="2">
         <f>0.001*(G12-$C$19+$C$20)</f>
-        <v>3.6000000000000016E-3</v>
+        <v>2.5399999999999993E-3</v>
       </c>
       <c r="M12" s="2">
         <f t="shared" ref="M12:M19" si="1">L12+$D$25</f>
-        <v>2.3920000000000004E-2</v>
+        <v>2.2860000000000002E-2</v>
       </c>
       <c r="N12" s="2">
         <f t="shared" ref="N12:N19" si="2">L12+$C$25</f>
-        <v>8.3820000000000006E-2</v>
+        <v>8.276E-2</v>
       </c>
       <c r="O12" s="2">
         <f t="shared" ref="O12:O19" si="3">L12+$C$25+$D$25</f>
-        <v>0.10414000000000001</v>
+        <v>0.10308</v>
       </c>
       <c r="P12" s="12">
         <f t="shared" ref="P12:P19" si="4">1/L12-1/M12-1/N12+1/O12</f>
-        <v>233.64388904923791</v>
+        <v>347.57432646943141</v>
       </c>
       <c r="Q12" s="12">
         <f t="shared" ref="Q12:Q19" si="5">$C$28*$C$29*P12*1000</f>
-        <v>48.54124107366092</v>
+        <v>232.96505556905876</v>
       </c>
       <c r="R12" s="12">
         <f t="shared" ref="R12:R19" si="6">$C$31*(LN(M12/L12)+LN(N12/O12))*1000</f>
-        <v>19.905727711070742</v>
+        <v>84.429838366889342</v>
       </c>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.2">
@@ -3562,45 +4978,43 @@
         <v>9</v>
       </c>
       <c r="G13" s="3">
-        <v>14.96</v>
+        <v>13.95</v>
       </c>
       <c r="H13" s="5">
-        <v>53.8</v>
-      </c>
-      <c r="I13" s="5">
-        <v>2.1</v>
-      </c>
+        <v>66.599999999999994</v>
+      </c>
+      <c r="I13" s="5"/>
       <c r="K13" s="18">
         <f t="shared" si="0"/>
-        <v>26.9</v>
+        <v>33.299999999999997</v>
       </c>
       <c r="L13" s="2">
         <f>0.001*(G13-$C$19+$C$20)</f>
-        <v>4.5900000000000021E-3</v>
+        <v>3.6299999999999991E-3</v>
       </c>
       <c r="M13" s="2">
         <f t="shared" si="1"/>
-        <v>2.4910000000000002E-2</v>
+        <v>2.3949999999999999E-2</v>
       </c>
       <c r="N13" s="2">
         <f t="shared" si="2"/>
-        <v>8.4809999999999997E-2</v>
+        <v>8.3849999999999994E-2</v>
       </c>
       <c r="O13" s="2">
         <f t="shared" si="3"/>
-        <v>0.10513</v>
+        <v>0.10417</v>
       </c>
       <c r="P13" s="12">
         <f t="shared" si="4"/>
-        <v>175.44137382096645</v>
+        <v>231.40207459137926</v>
       </c>
       <c r="Q13" s="12">
         <f t="shared" si="5"/>
-        <v>36.449239291437713</v>
+        <v>155.09947962372681</v>
       </c>
       <c r="R13" s="12">
         <f t="shared" si="6"/>
-        <v>17.530034090080751</v>
+        <v>71.284079709279737</v>
       </c>
     </row>
     <row r="14" spans="2:18" x14ac:dyDescent="0.2">
@@ -3614,45 +5028,43 @@
         <v>38</v>
       </c>
       <c r="G14" s="3">
-        <v>15.9</v>
+        <v>14.95</v>
       </c>
       <c r="H14" s="5">
-        <v>49.5</v>
-      </c>
-      <c r="I14" s="5">
-        <v>1.97</v>
-      </c>
+        <v>56.9</v>
+      </c>
+      <c r="I14" s="5"/>
       <c r="K14" s="18">
         <f t="shared" si="0"/>
-        <v>24.75</v>
+        <v>28.45</v>
       </c>
       <c r="L14" s="2">
         <f>0.001*(G14-$C$19+$C$20)</f>
-        <v>5.5300000000000011E-3</v>
+        <v>4.6299999999999987E-3</v>
       </c>
       <c r="M14" s="2">
         <f t="shared" si="1"/>
-        <v>2.5850000000000001E-2</v>
+        <v>2.495E-2</v>
       </c>
       <c r="N14" s="2">
         <f t="shared" si="2"/>
-        <v>8.5750000000000007E-2</v>
+        <v>8.4849999999999995E-2</v>
       </c>
       <c r="O14" s="2">
         <f t="shared" si="3"/>
-        <v>0.10607000000000001</v>
+        <v>0.10517</v>
       </c>
       <c r="P14" s="12">
         <f t="shared" si="4"/>
-        <v>139.91303568597857</v>
+        <v>173.62547217858773</v>
       </c>
       <c r="Q14" s="12">
         <f t="shared" si="5"/>
-        <v>29.067965022400237</v>
+        <v>116.37415278957937</v>
       </c>
       <c r="R14" s="12">
         <f t="shared" si="6"/>
-        <v>15.783145165346236</v>
+        <v>62.74073954929306</v>
       </c>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.2">
@@ -3666,45 +5078,43 @@
         <v>20</v>
       </c>
       <c r="G15" s="3">
-        <v>16.850000000000001</v>
+        <v>16.09</v>
       </c>
       <c r="H15" s="5">
-        <v>46.6</v>
-      </c>
-      <c r="I15" s="5">
-        <v>1.9</v>
-      </c>
+        <v>49.9</v>
+      </c>
+      <c r="I15" s="5"/>
       <c r="K15" s="18">
         <f t="shared" si="0"/>
-        <v>23.3</v>
+        <v>24.95</v>
       </c>
       <c r="L15" s="2">
         <f>0.001*(G15-$C$19+$C$20)</f>
-        <v>6.4800000000000023E-3</v>
+        <v>5.77E-3</v>
       </c>
       <c r="M15" s="2">
         <f t="shared" si="1"/>
-        <v>2.6800000000000004E-2</v>
+        <v>2.6090000000000002E-2</v>
       </c>
       <c r="N15" s="2">
         <f t="shared" si="2"/>
-        <v>8.6699999999999999E-2</v>
+        <v>8.5989999999999997E-2</v>
       </c>
       <c r="O15" s="2">
         <f t="shared" si="3"/>
-        <v>0.10702</v>
+        <v>0.10631</v>
       </c>
       <c r="P15" s="12">
         <f t="shared" si="4"/>
-        <v>114.81757728516916</v>
+        <v>132.75855728093455</v>
       </c>
       <c r="Q15" s="12">
         <f t="shared" si="5"/>
-        <v>23.854198460626375</v>
+        <v>88.982707636609817</v>
       </c>
       <c r="R15" s="12">
         <f t="shared" si="6"/>
-        <v>14.354485669151209</v>
+        <v>55.360532346029551</v>
       </c>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.2">
@@ -3718,45 +5128,43 @@
         <v>34</v>
       </c>
       <c r="G16" s="3">
-        <v>17.97</v>
+        <v>17.57</v>
       </c>
       <c r="H16" s="5">
-        <v>44.9</v>
-      </c>
-      <c r="I16" s="5">
-        <v>1.78</v>
-      </c>
+        <v>41.6</v>
+      </c>
+      <c r="I16" s="5"/>
       <c r="K16" s="18">
         <f t="shared" si="0"/>
-        <v>22.45</v>
+        <v>20.8</v>
       </c>
       <c r="L16" s="2">
         <f>0.001*(G16-$C$19+$C$20)</f>
-        <v>7.6E-3</v>
+        <v>7.2500000000000004E-3</v>
       </c>
       <c r="M16" s="2">
         <f t="shared" si="1"/>
-        <v>2.792E-2</v>
+        <v>2.7570000000000001E-2</v>
       </c>
       <c r="N16" s="2">
         <f t="shared" si="2"/>
-        <v>8.7819999999999995E-2</v>
+        <v>8.7470000000000006E-2</v>
       </c>
       <c r="O16" s="2">
         <f t="shared" si="3"/>
-        <v>0.10814</v>
+        <v>0.10779000000000001</v>
       </c>
       <c r="P16" s="12">
         <f t="shared" si="4"/>
-        <v>93.622672705112393</v>
+        <v>99.504532399361267</v>
       </c>
       <c r="Q16" s="12">
         <f t="shared" si="5"/>
-        <v>19.450800721698304</v>
+        <v>66.693875681951837</v>
       </c>
       <c r="R16" s="12">
         <f t="shared" si="6"/>
-        <v>12.976616008429373</v>
+        <v>48.106617928028541</v>
       </c>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.2">
@@ -3770,45 +5178,43 @@
         <v>0.16</v>
       </c>
       <c r="G17" s="3">
-        <v>18.66</v>
+        <v>18.72</v>
       </c>
       <c r="H17" s="5">
-        <v>43.5</v>
-      </c>
-      <c r="I17" s="5">
-        <v>2</v>
-      </c>
+        <v>37.1</v>
+      </c>
+      <c r="I17" s="5"/>
       <c r="K17" s="18">
         <f t="shared" si="0"/>
-        <v>21.75</v>
+        <v>18.55</v>
       </c>
       <c r="L17" s="2">
         <f>0.001*(G17-$C$19+$C$20)</f>
-        <v>8.2900000000000005E-3</v>
+        <v>8.3999999999999995E-3</v>
       </c>
       <c r="M17" s="2">
         <f t="shared" si="1"/>
-        <v>2.8610000000000003E-2</v>
+        <v>2.8720000000000002E-2</v>
       </c>
       <c r="N17" s="2">
         <f t="shared" si="2"/>
-        <v>8.8510000000000005E-2</v>
+        <v>8.8620000000000004E-2</v>
       </c>
       <c r="O17" s="2">
         <f t="shared" si="3"/>
-        <v>0.10883000000000001</v>
+        <v>0.10894000000000001</v>
       </c>
       <c r="P17" s="12">
         <f t="shared" si="4"/>
-        <v>83.564932496927185</v>
+        <v>82.123907824514134</v>
       </c>
       <c r="Q17" s="12">
         <f t="shared" si="5"/>
-        <v>17.36123101761379</v>
+        <v>55.044343879549523</v>
       </c>
       <c r="R17" s="12">
         <f t="shared" si="6"/>
-        <v>12.252162888712624</v>
+        <v>43.670292438337185</v>
       </c>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.2">
@@ -3816,51 +5222,49 @@
         <v>15</v>
       </c>
       <c r="C18" s="3">
-        <v>120</v>
+        <v>33.369999999999997</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>14</v>
       </c>
       <c r="G18" s="3">
-        <v>19.809999999999999</v>
+        <v>20.260000000000002</v>
       </c>
       <c r="H18" s="5">
-        <v>41.5</v>
-      </c>
-      <c r="I18" s="5">
-        <v>2</v>
-      </c>
+        <v>31.4</v>
+      </c>
+      <c r="I18" s="5"/>
       <c r="K18" s="18">
         <f t="shared" si="0"/>
-        <v>20.75</v>
+        <v>15.7</v>
       </c>
       <c r="L18" s="2">
         <f>0.001*(G18-$C$19+$C$20)</f>
-        <v>9.4400000000000005E-3</v>
+        <v>9.9400000000000009E-3</v>
       </c>
       <c r="M18" s="2">
         <f t="shared" si="1"/>
-        <v>2.9760000000000002E-2</v>
+        <v>3.0260000000000002E-2</v>
       </c>
       <c r="N18" s="2">
         <f t="shared" si="2"/>
-        <v>8.9660000000000004E-2</v>
+        <v>9.0160000000000004E-2</v>
       </c>
       <c r="O18" s="2">
         <f t="shared" si="3"/>
-        <v>0.10998000000000001</v>
+        <v>0.11048000000000001</v>
       </c>
       <c r="P18" s="12">
         <f t="shared" si="4"/>
-        <v>70.269369541779753</v>
+        <v>65.516714035863856</v>
       </c>
       <c r="Q18" s="12">
         <f t="shared" si="5"/>
-        <v>14.598979758905116</v>
+        <v>43.913211545587274</v>
       </c>
       <c r="R18" s="12">
         <f t="shared" si="6"/>
-        <v>11.206259923151407</v>
+        <v>38.849917880817657</v>
       </c>
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.2">
@@ -3868,47 +5272,47 @@
         <v>35</v>
       </c>
       <c r="C19" s="11">
-        <v>12.19</v>
+        <v>12.07</v>
       </c>
       <c r="D19" s="11"/>
       <c r="G19" s="3">
-        <v>20.62</v>
+        <v>23.06</v>
       </c>
       <c r="H19" s="5">
-        <v>40.299999999999997</v>
+        <v>25.1</v>
       </c>
       <c r="I19" s="5"/>
       <c r="K19" s="18">
         <f t="shared" si="0"/>
-        <v>20.149999999999999</v>
+        <v>12.55</v>
       </c>
       <c r="L19" s="2">
         <f>0.001*(G19-$C$19+$C$20)</f>
-        <v>1.0250000000000002E-2</v>
+        <v>1.2739999999999998E-2</v>
       </c>
       <c r="M19" s="2">
         <f t="shared" si="1"/>
-        <v>3.0570000000000003E-2</v>
+        <v>3.3059999999999999E-2</v>
       </c>
       <c r="N19" s="2">
         <f t="shared" si="2"/>
-        <v>9.0469999999999995E-2</v>
+        <v>9.2960000000000001E-2</v>
       </c>
       <c r="O19" s="2">
         <f t="shared" si="3"/>
-        <v>0.11079</v>
+        <v>0.11328000000000001</v>
       </c>
       <c r="P19" s="12">
         <f t="shared" si="4"/>
-        <v>62.821864170108057</v>
+        <v>46.315270399631615</v>
       </c>
       <c r="Q19" s="12">
         <f t="shared" si="5"/>
-        <v>13.051705592588204</v>
+        <v>31.043258148398106</v>
       </c>
       <c r="R19" s="12">
         <f t="shared" si="6"/>
-        <v>10.567409311644818</v>
+        <v>32.269976805909671</v>
       </c>
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.2">
@@ -3916,7 +5320,7 @@
         <v>34</v>
       </c>
       <c r="C20" s="11">
-        <v>1.82</v>
+        <v>1.75</v>
       </c>
       <c r="D20" s="11"/>
     </row>
@@ -3936,7 +5340,7 @@
       </c>
       <c r="C23" s="14">
         <f>2*H5*H7/C18</f>
-        <v>47166.666666666664</v>
+        <v>169613.42523224454</v>
       </c>
       <c r="D23" s="14"/>
     </row>
@@ -3972,7 +5376,7 @@
       </c>
       <c r="C28" s="15">
         <f>C11*D11*D24*C23</f>
-        <v>59359.250000000007</v>
+        <v>213458.49565477978</v>
       </c>
       <c r="D28" s="15"/>
     </row>
@@ -3981,7 +5385,7 @@
         <v>47</v>
       </c>
       <c r="C29" s="16">
-        <v>3.4999999999999999E-9</v>
+        <v>3.1399999999999999E-9</v>
       </c>
       <c r="D29" s="17"/>
     </row>
@@ -3991,7 +5395,7 @@
       </c>
       <c r="C31" s="16">
         <f>C28*C21/(2*PI())</f>
-        <v>1.1871850000000001E-2</v>
+        <v>4.2691699130955954E-2</v>
       </c>
       <c r="D31" s="17"/>
     </row>
@@ -4021,10 +5425,10 @@
   <sheetPr enableFormatConditionsCalculation="0">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B4:T35"/>
+  <dimension ref="B4:R35"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="C14" zoomScale="91" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView showGridLines="0" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="91" workbookViewId="0">
+      <selection activeCell="C29" sqref="C29:D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4046,7 +5450,7 @@
     <col min="20" max="20" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="4" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -4061,7 +5465,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="5" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
@@ -4074,7 +5478,7 @@
         <v>200000</v>
       </c>
     </row>
-    <row r="6" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="6" spans="2:18" x14ac:dyDescent="0.2">
       <c r="G6" s="1" t="s">
         <v>13</v>
       </c>
@@ -4082,7 +5486,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="7" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B7" s="4"/>
       <c r="C7" s="8" t="s">
         <v>2</v>
@@ -4100,7 +5504,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="8" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B8" s="1" t="s">
         <v>21</v>
       </c>
@@ -4111,7 +5515,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="9" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B9" s="1" t="s">
         <v>39</v>
       </c>
@@ -4122,7 +5526,7 @@
         <v>50.3</v>
       </c>
     </row>
-    <row r="10" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="10" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B10" s="1" t="s">
         <v>40</v>
       </c>
@@ -4139,7 +5543,7 @@
         <v>49</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="K10" s="8" t="s">
         <v>37</v>
@@ -4165,14 +5569,8 @@
       <c r="R10" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="S10" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="T10" s="8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="11" spans="2:20" x14ac:dyDescent="0.2">
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B11" s="1" t="s">
         <v>6</v>
       </c>
@@ -4217,22 +5615,14 @@
       </c>
       <c r="Q11" s="12">
         <f>$C$28*$C$29*P11*1000</f>
-        <v>233.74770407136475</v>
+        <v>259.30259823435705</v>
       </c>
       <c r="R11" s="12">
         <f>$C$31*(LN(M11/L11)+LN(N11/O11))*1000</f>
-        <v>119.31118788290024</v>
-      </c>
-      <c r="S11" s="12">
-        <f>$C$31*LN(M11/L11)*1000</f>
-        <v>143.917273043812</v>
-      </c>
-      <c r="T11" s="12">
-        <f>$C$31*(LN(N11/O11))*1000</f>
-        <v>-24.606085160911764</v>
-      </c>
-    </row>
-    <row r="12" spans="2:20" x14ac:dyDescent="0.2">
+        <v>118.02365707840856</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
         <v>7</v>
       </c>
@@ -4240,7 +5630,7 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="D12" s="3">
-        <v>3</v>
+        <v>2.71</v>
       </c>
       <c r="G12" s="3">
         <v>13.49</v>
@@ -4248,8 +5638,8 @@
       <c r="H12" s="5">
         <v>181.6</v>
       </c>
-      <c r="I12" s="5" t="s">
-        <v>14</v>
+      <c r="I12" s="5">
+        <v>182.8</v>
       </c>
       <c r="K12" s="18">
         <f t="shared" ref="K12:K21" si="0">H12/2</f>
@@ -4277,22 +5667,14 @@
       </c>
       <c r="Q12" s="12">
         <f t="shared" ref="Q12:Q21" si="5">$C$28*$C$29*P12*1000</f>
-        <v>208.51172916540338</v>
+        <v>231.30765433495102</v>
       </c>
       <c r="R12" s="12">
         <f t="shared" ref="R12:R21" si="6">$C$31*(LN(M12/L12)+LN(N12/O12))*1000</f>
-        <v>114.74008185769046</v>
-      </c>
-      <c r="S12" s="12">
-        <f t="shared" ref="S12:S21" si="7">$C$31*LN(M12/L12)*1000</f>
-        <v>139.28000935284481</v>
-      </c>
-      <c r="T12" s="12">
-        <f t="shared" ref="T12:T21" si="8">$C$31*(LN(N12/O12))*1000</f>
-        <v>-24.539927495154359</v>
-      </c>
-    </row>
-    <row r="13" spans="2:20" x14ac:dyDescent="0.2">
+        <v>113.5018795354852</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B13" s="1" t="s">
         <v>8</v>
       </c>
@@ -4337,22 +5719,14 @@
       </c>
       <c r="Q13" s="12">
         <f t="shared" si="5"/>
-        <v>139.77409466885595</v>
+        <v>155.05515255210324</v>
       </c>
       <c r="R13" s="12">
         <f t="shared" si="6"/>
-        <v>99.208940538776375</v>
-      </c>
-      <c r="S13" s="12">
-        <f t="shared" si="7"/>
-        <v>123.46116442144547</v>
-      </c>
-      <c r="T13" s="12">
-        <f t="shared" si="8"/>
-        <v>-24.252223882669099</v>
-      </c>
-    </row>
-    <row r="14" spans="2:20" x14ac:dyDescent="0.2">
+        <v>98.138340461019837</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B14" s="1" t="s">
         <v>10</v>
       </c>
@@ -4397,22 +5771,14 @@
       </c>
       <c r="Q14" s="12">
         <f t="shared" si="5"/>
-        <v>85.944625607619429</v>
+        <v>95.34067858707526</v>
       </c>
       <c r="R14" s="12">
         <f t="shared" si="6"/>
-        <v>81.550168145515499</v>
-      </c>
-      <c r="S14" s="12">
-        <f t="shared" si="7"/>
-        <v>105.30879882626297</v>
-      </c>
-      <c r="T14" s="12">
-        <f t="shared" si="8"/>
-        <v>-23.75863068074748</v>
-      </c>
-    </row>
-    <row r="15" spans="2:20" x14ac:dyDescent="0.2">
+        <v>80.670130359772557</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B15" s="1" t="s">
         <v>11</v>
       </c>
@@ -4428,8 +5794,8 @@
       <c r="H15" s="5">
         <v>98.9</v>
       </c>
-      <c r="I15" s="5" t="s">
-        <v>14</v>
+      <c r="I15" s="5">
+        <v>102.2</v>
       </c>
       <c r="K15" s="18">
         <f t="shared" si="0"/>
@@ -4457,22 +5823,14 @@
       </c>
       <c r="Q15" s="12">
         <f t="shared" si="5"/>
-        <v>63.481971428672388</v>
+        <v>70.422253762408289</v>
       </c>
       <c r="R15" s="12">
         <f t="shared" si="6"/>
-        <v>71.388468670187109</v>
-      </c>
-      <c r="S15" s="12">
-        <f t="shared" si="7"/>
-        <v>94.743320673049396</v>
-      </c>
-      <c r="T15" s="12">
-        <f t="shared" si="8"/>
-        <v>-23.354852002862284</v>
-      </c>
-    </row>
-    <row r="16" spans="2:20" x14ac:dyDescent="0.2">
+        <v>70.618089511875766</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B16" s="1" t="s">
         <v>12</v>
       </c>
@@ -4517,22 +5875,14 @@
       </c>
       <c r="Q16" s="12">
         <f t="shared" si="5"/>
-        <v>40.179636596743499</v>
+        <v>44.572348665580698</v>
       </c>
       <c r="R16" s="12">
         <f t="shared" si="6"/>
-        <v>57.479571357800687</v>
-      </c>
-      <c r="S16" s="12">
-        <f t="shared" si="7"/>
-        <v>80.06560496236122</v>
-      </c>
-      <c r="T16" s="12">
-        <f t="shared" si="8"/>
-        <v>-22.586033604560527</v>
-      </c>
-    </row>
-    <row r="17" spans="2:20" x14ac:dyDescent="0.2">
+        <v>56.85928821365178</v>
+      </c>
+    </row>
+    <row r="17" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
         <v>19</v>
       </c>
@@ -4577,27 +5927,19 @@
       </c>
       <c r="Q17" s="12">
         <f t="shared" si="5"/>
-        <v>34.428795512471829</v>
+        <v>38.192786388771111</v>
       </c>
       <c r="R17" s="12">
         <f t="shared" si="6"/>
-        <v>53.203774046832798</v>
-      </c>
-      <c r="S17" s="12">
-        <f t="shared" si="7"/>
-        <v>75.484972826376108</v>
-      </c>
-      <c r="T17" s="12">
-        <f t="shared" si="8"/>
-        <v>-22.28119877954331</v>
-      </c>
-    </row>
-    <row r="18" spans="2:20" x14ac:dyDescent="0.2">
+        <v>52.62963260028426</v>
+      </c>
+    </row>
+    <row r="18" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B18" s="1" t="s">
         <v>15</v>
       </c>
       <c r="C18" s="3">
-        <v>33</v>
+        <v>33.36</v>
       </c>
       <c r="D18" s="2" t="s">
         <v>14</v>
@@ -4637,22 +5979,14 @@
       </c>
       <c r="Q18" s="12">
         <f t="shared" si="5"/>
-        <v>27.94351018531616</v>
+        <v>30.998485412410727</v>
       </c>
       <c r="R18" s="12">
         <f t="shared" si="6"/>
-        <v>47.778537612650588</v>
-      </c>
-      <c r="S18" s="12">
-        <f t="shared" si="7"/>
-        <v>69.611632491480378</v>
-      </c>
-      <c r="T18" s="12">
-        <f t="shared" si="8"/>
-        <v>-21.833094878829794</v>
-      </c>
-    </row>
-    <row r="19" spans="2:20" x14ac:dyDescent="0.2">
+        <v>47.262941883017689</v>
+      </c>
+    </row>
+    <row r="19" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B19" s="1" t="s">
         <v>35</v>
       </c>
@@ -4695,22 +6029,14 @@
       </c>
       <c r="Q19" s="12">
         <f t="shared" si="5"/>
-        <v>19.092214567288263</v>
+        <v>21.179505753922687</v>
       </c>
       <c r="R19" s="12">
         <f t="shared" si="6"/>
-        <v>38.929315794891707</v>
-      </c>
-      <c r="S19" s="12">
-        <f t="shared" si="7"/>
-        <v>59.841716833654175</v>
-      </c>
-      <c r="T19" s="12">
-        <f t="shared" si="8"/>
-        <v>-20.912401038762464</v>
-      </c>
-    </row>
-    <row r="20" spans="2:20" x14ac:dyDescent="0.2">
+        <v>38.509215264731019</v>
+      </c>
+    </row>
+    <row r="20" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B20" s="1" t="s">
         <v>34</v>
       </c>
@@ -4753,22 +6079,14 @@
       </c>
       <c r="Q20" s="12">
         <f t="shared" si="5"/>
-        <v>14.740380760103472</v>
+        <v>16.351899776913349</v>
       </c>
       <c r="R20" s="12">
         <f t="shared" si="6"/>
-        <v>33.682477319565088</v>
-      </c>
-      <c r="S20" s="12">
-        <f t="shared" si="7"/>
-        <v>53.900445551402399</v>
-      </c>
-      <c r="T20" s="12">
-        <f t="shared" si="8"/>
-        <v>-20.217968231837315</v>
-      </c>
-    </row>
-    <row r="21" spans="2:20" x14ac:dyDescent="0.2">
+        <v>33.318997348490647</v>
+      </c>
+    </row>
+    <row r="21" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B21" s="1" t="s">
         <v>48</v>
       </c>
@@ -4799,51 +6117,43 @@
         <v>0.10443</v>
       </c>
       <c r="N21" s="2">
-        <f t="shared" ref="N21" si="9">L21+$C$25</f>
+        <f t="shared" ref="N21" si="7">L21+$C$25</f>
         <v>0.12406</v>
       </c>
       <c r="O21" s="2">
-        <f t="shared" ref="O21" si="10">L21+$C$25+$D$25</f>
+        <f t="shared" ref="O21" si="8">L21+$C$25+$D$25</f>
         <v>0.18465000000000001</v>
       </c>
       <c r="P21" s="12">
-        <f t="shared" ref="P21" si="11">1/L21-1/M21-1/N21+1/O21</f>
+        <f t="shared" ref="P21" si="9">1/L21-1/M21-1/N21+1/O21</f>
         <v>10.589461982292516</v>
       </c>
       <c r="Q21" s="12">
         <f t="shared" si="5"/>
-        <v>6.6404850015604477</v>
+        <v>7.3664681382932269</v>
       </c>
       <c r="R21" s="12">
         <f t="shared" si="6"/>
-        <v>21.064366374712304</v>
-      </c>
-      <c r="S21" s="12">
-        <f t="shared" si="7"/>
-        <v>38.877896362213782</v>
-      </c>
-      <c r="T21" s="12">
-        <f t="shared" si="8"/>
-        <v>-17.813529987501482</v>
-      </c>
-    </row>
-    <row r="22" spans="2:20" x14ac:dyDescent="0.2">
+        <v>20.837053068510379</v>
+      </c>
+    </row>
+    <row r="22" spans="2:18" x14ac:dyDescent="0.2">
       <c r="H22" s="11" t="s">
         <v>55</v>
       </c>
       <c r="I22" s="11"/>
     </row>
-    <row r="23" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B23" s="1" t="s">
         <v>32</v>
       </c>
       <c r="C23" s="14">
         <f>2*H5*H7/C18</f>
-        <v>89333.333333333328</v>
+        <v>88369.304556354924</v>
       </c>
       <c r="D23" s="14"/>
     </row>
-    <row r="24" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B24" s="1" t="s">
         <v>41</v>
       </c>
@@ -4856,7 +6166,7 @@
         <v>5.0140000000000004E-2</v>
       </c>
     </row>
-    <row r="25" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B25" s="1" t="s">
         <v>42</v>
       </c>
@@ -4869,32 +6179,32 @@
         <v>6.0590000000000005E-2</v>
       </c>
     </row>
-    <row r="28" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B28" s="1" t="s">
         <v>46</v>
       </c>
       <c r="C28" s="15">
         <f>C11*D11*D24*C23</f>
-        <v>223958.66666666666</v>
+        <v>221541.84652278179</v>
       </c>
       <c r="D28" s="15"/>
     </row>
-    <row r="29" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B29" s="1" t="s">
         <v>47</v>
       </c>
       <c r="C29" s="16">
-        <v>2.7999999999999998E-9</v>
+        <v>3.1399999999999999E-9</v>
       </c>
       <c r="D29" s="17"/>
     </row>
-    <row r="31" spans="2:20" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B31" s="1" t="s">
         <v>45</v>
       </c>
       <c r="C31" s="16">
         <f>C28*C21/(2*PI())</f>
-        <v>4.4791733333333326E-2</v>
+        <v>4.4308369304556366E-2</v>
       </c>
       <c r="D31" s="17"/>
     </row>
@@ -4918,13 +6228,997 @@
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="40" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup scale="45" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr enableFormatConditionsCalculation="0">
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="B4:R35"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A8" zoomScale="91" zoomScaleNormal="91" zoomScalePageLayoutView="91" workbookViewId="0">
+      <selection activeCell="Q43" sqref="Q43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.83203125" customWidth="1"/>
+    <col min="4" max="4" width="13.5" customWidth="1"/>
+    <col min="5" max="5" width="5.33203125" customWidth="1"/>
+    <col min="6" max="6" width="3.83203125" customWidth="1"/>
+    <col min="7" max="7" width="17.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13" customWidth="1"/>
+    <col min="11" max="11" width="19" customWidth="1"/>
+    <col min="15" max="15" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="19">
+        <v>42431</v>
+      </c>
+      <c r="D4" s="19"/>
+      <c r="G4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="H4" s="13" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="G5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="5">
+        <v>200000</v>
+      </c>
+    </row>
+    <row r="6" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="G6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B7" s="4"/>
+      <c r="C7" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="3">
+        <v>7.38</v>
+      </c>
+      <c r="I7" s="24" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B8" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D8" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B9" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C9" s="5">
+        <v>80.069999999999993</v>
+      </c>
+      <c r="D9" s="5">
+        <v>50.36</v>
+      </c>
+    </row>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C10" s="5">
+        <v>80.38</v>
+      </c>
+      <c r="D10" s="5">
+        <v>40.85</v>
+      </c>
+      <c r="G10" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="H10" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="I10" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="K10" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="L10" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="M10" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="N10" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="O10" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="P10" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="Q10" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="R10" s="8" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="11" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B11" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C11" s="3">
+        <v>5</v>
+      </c>
+      <c r="D11" s="3">
+        <v>10</v>
+      </c>
+      <c r="G11" s="3">
+        <v>12.41</v>
+      </c>
+      <c r="H11" s="5">
+        <v>211</v>
+      </c>
+      <c r="I11" s="5"/>
+      <c r="K11" s="18">
+        <f>H11/2</f>
+        <v>105.5</v>
+      </c>
+      <c r="L11" s="2">
+        <f>0.001*(G11-$C$19+$C$20)</f>
+        <v>1.98E-3</v>
+      </c>
+      <c r="M11" s="2">
+        <f>L11+$D$25</f>
+        <v>4.2670000000000007E-2</v>
+      </c>
+      <c r="N11" s="2">
+        <f>L11+$C$25</f>
+        <v>8.2199999999999995E-2</v>
+      </c>
+      <c r="O11" s="2">
+        <f>L11+$C$25+$D$25</f>
+        <v>0.12289</v>
+      </c>
+      <c r="P11" s="12">
+        <f>1/L11-1/M11-1/N11+1/O11</f>
+        <v>477.58674445389221</v>
+      </c>
+      <c r="Q11" s="12">
+        <f>$C$28*$C$29*P11*1000</f>
+        <v>33.307799757689608</v>
+      </c>
+      <c r="R11" s="12">
+        <f>$C$31*(LN(M11/L11)+LN(N11/O11))*1000</f>
+        <v>118.52855037796115</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B12" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="3">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="D12" s="3">
+        <v>2.64</v>
+      </c>
+      <c r="G12" s="3">
+        <v>13.14</v>
+      </c>
+      <c r="H12" s="5">
+        <v>182</v>
+      </c>
+      <c r="I12" s="5"/>
+      <c r="K12" s="18">
+        <f t="shared" ref="K12:K22" si="0">H12/2</f>
+        <v>91</v>
+      </c>
+      <c r="L12" s="2">
+        <f>0.001*(G12-$C$19+$C$20)</f>
+        <v>2.7100000000000006E-3</v>
+      </c>
+      <c r="M12" s="2">
+        <f t="shared" ref="M12:M26" si="1">L12+$D$25</f>
+        <v>4.3400000000000008E-2</v>
+      </c>
+      <c r="N12" s="2">
+        <f t="shared" ref="N12:N22" si="2">L12+$C$25</f>
+        <v>8.2930000000000004E-2</v>
+      </c>
+      <c r="O12" s="2">
+        <f t="shared" ref="O12:O22" si="3">L12+$C$25+$D$25</f>
+        <v>0.12362000000000001</v>
+      </c>
+      <c r="P12" s="12">
+        <f t="shared" ref="P12:P22" si="4">1/L12-1/M12-1/N12+1/O12</f>
+        <v>341.993158845697</v>
+      </c>
+      <c r="Q12" s="12">
+        <f t="shared" ref="Q12:Q26" si="5">$C$28*$C$29*P12*1000</f>
+        <v>23.851247518097601</v>
+      </c>
+      <c r="R12" s="12">
+        <f t="shared" ref="R12:R22" si="6">$C$31*(LN(M12/L12)+LN(N12/O12))*1000</f>
+        <v>105.46995690016124</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B13" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" s="3">
+        <v>13.77</v>
+      </c>
+      <c r="H13" s="5">
+        <v>164</v>
+      </c>
+      <c r="I13" s="5"/>
+      <c r="K13" s="18">
+        <f t="shared" si="0"/>
+        <v>82</v>
+      </c>
+      <c r="L13" s="2">
+        <f>0.001*(G13-$C$19+$C$20)</f>
+        <v>3.3399999999999997E-3</v>
+      </c>
+      <c r="M13" s="2">
+        <f t="shared" si="1"/>
+        <v>4.4030000000000007E-2</v>
+      </c>
+      <c r="N13" s="2">
+        <f t="shared" si="2"/>
+        <v>8.3559999999999995E-2</v>
+      </c>
+      <c r="O13" s="2">
+        <f t="shared" si="3"/>
+        <v>0.12425</v>
+      </c>
+      <c r="P13" s="12">
+        <f t="shared" si="4"/>
+        <v>272.77025138558002</v>
+      </c>
+      <c r="Q13" s="12">
+        <f t="shared" si="5"/>
+        <v>19.023511474118578</v>
+      </c>
+      <c r="R13" s="12">
+        <f t="shared" si="6"/>
+        <v>96.93543117882129</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="G14" s="3">
+        <v>14.48</v>
+      </c>
+      <c r="H14" s="5">
+        <v>148</v>
+      </c>
+      <c r="I14" s="5"/>
+      <c r="K14" s="18">
+        <f t="shared" si="0"/>
+        <v>74</v>
+      </c>
+      <c r="L14" s="2">
+        <f>0.001*(G14-$C$19+$C$20)</f>
+        <v>4.0500000000000006E-3</v>
+      </c>
+      <c r="M14" s="2">
+        <f t="shared" si="1"/>
+        <v>4.4740000000000002E-2</v>
+      </c>
+      <c r="N14" s="2">
+        <f t="shared" si="2"/>
+        <v>8.4269999999999998E-2</v>
+      </c>
+      <c r="O14" s="2">
+        <f t="shared" si="3"/>
+        <v>0.12496</v>
+      </c>
+      <c r="P14" s="12">
+        <f t="shared" si="4"/>
+        <v>220.69815843301649</v>
+      </c>
+      <c r="Q14" s="12">
+        <f t="shared" si="5"/>
+        <v>15.391905561330871</v>
+      </c>
+      <c r="R14" s="12">
+        <f t="shared" si="6"/>
+        <v>89.206681433470891</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="G15" s="3">
+        <v>15.3</v>
+      </c>
+      <c r="H15" s="5">
+        <v>134</v>
+      </c>
+      <c r="I15" s="5"/>
+      <c r="K15" s="18">
+        <f t="shared" si="0"/>
+        <v>67</v>
+      </c>
+      <c r="L15" s="2">
+        <f>0.001*(G15-$C$19+$C$20)</f>
+        <v>4.8700000000000011E-3</v>
+      </c>
+      <c r="M15" s="2">
+        <f t="shared" si="1"/>
+        <v>4.5560000000000003E-2</v>
+      </c>
+      <c r="N15" s="2">
+        <f t="shared" si="2"/>
+        <v>8.5089999999999999E-2</v>
+      </c>
+      <c r="O15" s="2">
+        <f t="shared" si="3"/>
+        <v>0.12578</v>
+      </c>
+      <c r="P15" s="12">
+        <f t="shared" si="4"/>
+        <v>179.58785815478348</v>
+      </c>
+      <c r="Q15" s="12">
+        <f t="shared" si="5"/>
+        <v>12.52479573144724</v>
+      </c>
+      <c r="R15" s="12">
+        <f t="shared" si="6"/>
+        <v>81.962767474640401</v>
+      </c>
+    </row>
+    <row r="16" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B16" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="3">
+        <v>34</v>
+      </c>
+      <c r="D16" s="3">
+        <v>34</v>
+      </c>
+      <c r="G16" s="3">
+        <v>16.13</v>
+      </c>
+      <c r="H16" s="5">
+        <v>120</v>
+      </c>
+      <c r="I16" s="5"/>
+      <c r="K16" s="18">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="L16" s="2">
+        <f>0.001*(G16-$C$19+$C$20)</f>
+        <v>5.6999999999999993E-3</v>
+      </c>
+      <c r="M16" s="2">
+        <f t="shared" si="1"/>
+        <v>4.6390000000000001E-2</v>
+      </c>
+      <c r="N16" s="2">
+        <f t="shared" si="2"/>
+        <v>8.5919999999999996E-2</v>
+      </c>
+      <c r="O16" s="2">
+        <f t="shared" si="3"/>
+        <v>0.12661</v>
+      </c>
+      <c r="P16" s="12">
+        <f t="shared" si="4"/>
+        <v>150.14176315695661</v>
+      </c>
+      <c r="Q16" s="12">
+        <f t="shared" si="5"/>
+        <v>10.471169563587358</v>
+      </c>
+      <c r="R16" s="12">
+        <f t="shared" si="6"/>
+        <v>75.913059061936025</v>
+      </c>
+    </row>
+    <row r="17" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B17" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="3">
+        <v>0.16</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0.16</v>
+      </c>
+      <c r="G17" s="3">
+        <v>17.579999999999998</v>
+      </c>
+      <c r="H17" s="5">
+        <v>105</v>
+      </c>
+      <c r="I17" s="5"/>
+      <c r="K17" s="18">
+        <f t="shared" si="0"/>
+        <v>52.5</v>
+      </c>
+      <c r="L17" s="2">
+        <f>0.001*(G17-$C$19+$C$20)</f>
+        <v>7.1499999999999984E-3</v>
+      </c>
+      <c r="M17" s="2">
+        <f t="shared" si="1"/>
+        <v>4.7840000000000001E-2</v>
+      </c>
+      <c r="N17" s="2">
+        <f t="shared" si="2"/>
+        <v>8.7370000000000003E-2</v>
+      </c>
+      <c r="O17" s="2">
+        <f t="shared" si="3"/>
+        <v>0.12806000000000001</v>
+      </c>
+      <c r="P17" s="12">
+        <f t="shared" si="4"/>
+        <v>115.32039314836364</v>
+      </c>
+      <c r="Q17" s="12">
+        <f t="shared" si="5"/>
+        <v>8.0426615846633194</v>
+      </c>
+      <c r="R17" s="12">
+        <f t="shared" si="6"/>
+        <v>67.44985663207089</v>
+      </c>
+    </row>
+    <row r="18" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B18" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C18" s="3">
+        <v>33.36</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18" s="3">
+        <v>19.489999999999998</v>
+      </c>
+      <c r="H18" s="5">
+        <v>87.5</v>
+      </c>
+      <c r="I18" s="5"/>
+      <c r="K18" s="18">
+        <f t="shared" si="0"/>
+        <v>43.75</v>
+      </c>
+      <c r="L18" s="2">
+        <f>0.001*(G18-$C$19+$C$20)</f>
+        <v>9.0599999999999986E-3</v>
+      </c>
+      <c r="M18" s="2">
+        <f t="shared" si="1"/>
+        <v>4.9750000000000003E-2</v>
+      </c>
+      <c r="N18" s="2">
+        <f t="shared" si="2"/>
+        <v>8.9279999999999998E-2</v>
+      </c>
+      <c r="O18" s="2">
+        <f t="shared" si="3"/>
+        <v>0.12997</v>
+      </c>
+      <c r="P18" s="12">
+        <f t="shared" si="4"/>
+        <v>86.768139829729677</v>
+      </c>
+      <c r="Q18" s="12">
+        <f t="shared" si="5"/>
+        <v>6.0513736203054593</v>
+      </c>
+      <c r="R18" s="12">
+        <f t="shared" si="6"/>
+        <v>58.974767894161047</v>
+      </c>
+    </row>
+    <row r="19" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B19" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="11">
+        <v>12.41</v>
+      </c>
+      <c r="D19" s="11"/>
+      <c r="G19" s="3">
+        <v>20.95</v>
+      </c>
+      <c r="H19" s="5">
+        <v>77.7</v>
+      </c>
+      <c r="I19" s="5"/>
+      <c r="K19" s="18">
+        <f t="shared" si="0"/>
+        <v>38.85</v>
+      </c>
+      <c r="L19" s="2">
+        <f>0.001*(G19-$C$19+$C$20)</f>
+        <v>1.052E-2</v>
+      </c>
+      <c r="M19" s="2">
+        <f t="shared" si="1"/>
+        <v>5.1210000000000006E-2</v>
+      </c>
+      <c r="N19" s="2">
+        <f t="shared" si="2"/>
+        <v>9.0740000000000001E-2</v>
+      </c>
+      <c r="O19" s="2">
+        <f t="shared" si="3"/>
+        <v>0.13142999999999999</v>
+      </c>
+      <c r="P19" s="12">
+        <f t="shared" si="4"/>
+        <v>72.117712996229287</v>
+      </c>
+      <c r="Q19" s="12">
+        <f t="shared" si="5"/>
+        <v>5.0296252384635425</v>
+      </c>
+      <c r="R19" s="12">
+        <f t="shared" si="6"/>
+        <v>53.846976453767681</v>
+      </c>
+    </row>
+    <row r="20" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B20" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="11">
+        <v>1.98</v>
+      </c>
+      <c r="D20" s="11"/>
+      <c r="G20" s="3">
+        <v>23.66</v>
+      </c>
+      <c r="H20" s="5">
+        <v>63.8</v>
+      </c>
+      <c r="I20" s="5"/>
+      <c r="K20" s="18">
+        <f t="shared" si="0"/>
+        <v>31.9</v>
+      </c>
+      <c r="L20" s="2">
+        <f>0.001*(G20-$C$19+$C$20)</f>
+        <v>1.323E-2</v>
+      </c>
+      <c r="M20" s="2">
+        <f t="shared" si="1"/>
+        <v>5.3920000000000003E-2</v>
+      </c>
+      <c r="N20" s="2">
+        <f t="shared" si="2"/>
+        <v>9.3450000000000005E-2</v>
+      </c>
+      <c r="O20" s="2">
+        <f t="shared" si="3"/>
+        <v>0.13414000000000001</v>
+      </c>
+      <c r="P20" s="12">
+        <f t="shared" si="4"/>
+        <v>53.7937840968074</v>
+      </c>
+      <c r="Q20" s="12">
+        <f t="shared" si="5"/>
+        <v>3.7516798983892867</v>
+      </c>
+      <c r="R20" s="12">
+        <f t="shared" si="6"/>
+        <v>46.356453244568932</v>
+      </c>
+    </row>
+    <row r="21" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B21" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="14">
+        <f>4*PI()*0.0000001</f>
+        <v>1.2566370614359173E-6</v>
+      </c>
+      <c r="D21" s="14"/>
+      <c r="G21" s="3">
+        <v>25.96</v>
+      </c>
+      <c r="H21" s="5">
+        <v>54.6</v>
+      </c>
+      <c r="I21" s="5"/>
+      <c r="K21" s="18">
+        <f t="shared" si="0"/>
+        <v>27.3</v>
+      </c>
+      <c r="L21" s="2">
+        <f>0.001*(G21-$C$19+$C$20)</f>
+        <v>1.5530000000000002E-2</v>
+      </c>
+      <c r="M21" s="2">
+        <f t="shared" si="1"/>
+        <v>5.6220000000000006E-2</v>
+      </c>
+      <c r="N21" s="2">
+        <f t="shared" si="2"/>
+        <v>9.5750000000000002E-2</v>
+      </c>
+      <c r="O21" s="2">
+        <f t="shared" si="3"/>
+        <v>0.13644000000000001</v>
+      </c>
+      <c r="P21" s="12">
+        <f t="shared" si="4"/>
+        <v>43.489600738557577</v>
+      </c>
+      <c r="Q21" s="12">
+        <f t="shared" si="5"/>
+        <v>3.0330467287112759</v>
+      </c>
+      <c r="R21" s="12">
+        <f t="shared" si="6"/>
+        <v>41.416666949093461</v>
+      </c>
+    </row>
+    <row r="22" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="G22" s="3">
+        <v>28.24</v>
+      </c>
+      <c r="H22" s="5">
+        <v>47.4</v>
+      </c>
+      <c r="I22" s="5"/>
+      <c r="K22" s="22">
+        <f t="shared" si="0"/>
+        <v>23.7</v>
+      </c>
+      <c r="L22" s="20">
+        <f>0.001*(G22-$C$19+$C$20)</f>
+        <v>1.7809999999999999E-2</v>
+      </c>
+      <c r="M22" s="20">
+        <f t="shared" si="1"/>
+        <v>5.8500000000000003E-2</v>
+      </c>
+      <c r="N22" s="20">
+        <f t="shared" si="2"/>
+        <v>9.8030000000000006E-2</v>
+      </c>
+      <c r="O22" s="20">
+        <f t="shared" si="3"/>
+        <v>0.13872000000000001</v>
+      </c>
+      <c r="P22" s="21">
+        <f t="shared" si="4"/>
+        <v>36.062021205845198</v>
+      </c>
+      <c r="Q22" s="21">
+        <f t="shared" si="5"/>
+        <v>2.5150333319140326</v>
+      </c>
+      <c r="R22" s="21">
+        <f t="shared" si="6"/>
+        <v>37.406646245810649</v>
+      </c>
+    </row>
+    <row r="23" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B23" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C23" s="14">
+        <f>2*H5*H7/C18</f>
+        <v>88489.208633093527</v>
+      </c>
+      <c r="D23" s="14"/>
+      <c r="G23" s="3">
+        <v>30.08</v>
+      </c>
+      <c r="H23" s="5">
+        <v>41.6</v>
+      </c>
+      <c r="I23" s="5"/>
+      <c r="K23" s="22">
+        <f t="shared" ref="K23:K26" si="7">H23/2</f>
+        <v>20.8</v>
+      </c>
+      <c r="L23" s="20">
+        <f t="shared" ref="L23:L26" si="8">0.001*(G23-$C$19+$C$20)</f>
+        <v>1.9649999999999997E-2</v>
+      </c>
+      <c r="M23" s="20">
+        <f t="shared" si="1"/>
+        <v>6.0340000000000005E-2</v>
+      </c>
+      <c r="N23" s="20">
+        <f t="shared" ref="N23:N26" si="9">L23+$C$25</f>
+        <v>9.987E-2</v>
+      </c>
+      <c r="O23" s="20">
+        <f t="shared" ref="O23:O26" si="10">L23+$C$25+$D$25</f>
+        <v>0.14056000000000002</v>
+      </c>
+      <c r="P23" s="21">
+        <f t="shared" ref="P23:P26" si="11">1/L23-1/M23-1/N23+1/O23</f>
+        <v>31.419213472630197</v>
+      </c>
+      <c r="Q23" s="21">
+        <f t="shared" si="5"/>
+        <v>2.1912351694080638</v>
+      </c>
+      <c r="R23" s="21">
+        <f t="shared" ref="R23:R26" si="12">$C$31*(LN(M23/L23)+LN(N23/O23))*1000</f>
+        <v>34.655621785596665</v>
+      </c>
+    </row>
+    <row r="24" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B24" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C24" s="2">
+        <f>(C9-C17)*0.001</f>
+        <v>7.9909999999999995E-2</v>
+      </c>
+      <c r="D24" s="2">
+        <f>(D9-D17)*0.001</f>
+        <v>5.0200000000000002E-2</v>
+      </c>
+      <c r="G24" s="3">
+        <v>34.479999999999997</v>
+      </c>
+      <c r="H24" s="5">
+        <v>34</v>
+      </c>
+      <c r="I24" s="5"/>
+      <c r="K24" s="22">
+        <f t="shared" si="7"/>
+        <v>17</v>
+      </c>
+      <c r="L24" s="20">
+        <f t="shared" si="8"/>
+        <v>2.4049999999999998E-2</v>
+      </c>
+      <c r="M24" s="20">
+        <f t="shared" si="1"/>
+        <v>6.4740000000000006E-2</v>
+      </c>
+      <c r="N24" s="20">
+        <f t="shared" si="9"/>
+        <v>0.10427</v>
+      </c>
+      <c r="O24" s="20">
+        <f t="shared" si="10"/>
+        <v>0.14496000000000001</v>
+      </c>
+      <c r="P24" s="21">
+        <f t="shared" si="11"/>
+        <v>23.44160909995653</v>
+      </c>
+      <c r="Q24" s="21">
+        <f t="shared" si="5"/>
+        <v>1.6348620035344521</v>
+      </c>
+      <c r="R24" s="21">
+        <f t="shared" si="12"/>
+        <v>29.35245359646682</v>
+      </c>
+    </row>
+    <row r="25" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B25" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C25" s="2">
+        <f>(C10-C17)*0.001</f>
+        <v>8.022E-2</v>
+      </c>
+      <c r="D25" s="2">
+        <f>(D10-D17)*0.001</f>
+        <v>4.0690000000000004E-2</v>
+      </c>
+      <c r="G25" s="3">
+        <v>40.65</v>
+      </c>
+      <c r="H25" s="5">
+        <v>26.2</v>
+      </c>
+      <c r="I25" s="5"/>
+      <c r="K25" s="22">
+        <f t="shared" si="7"/>
+        <v>13.1</v>
+      </c>
+      <c r="L25" s="20">
+        <f t="shared" si="8"/>
+        <v>3.022E-2</v>
+      </c>
+      <c r="M25" s="20">
+        <f t="shared" si="1"/>
+        <v>7.0910000000000001E-2</v>
+      </c>
+      <c r="N25" s="20">
+        <f t="shared" si="9"/>
+        <v>0.11044</v>
+      </c>
+      <c r="O25" s="20">
+        <f t="shared" si="10"/>
+        <v>0.15112999999999999</v>
+      </c>
+      <c r="P25" s="21">
+        <f t="shared" si="11"/>
+        <v>16.550414755462405</v>
+      </c>
+      <c r="Q25" s="21">
+        <f t="shared" si="5"/>
+        <v>1.1542571207917465</v>
+      </c>
+      <c r="R25" s="21">
+        <f t="shared" si="12"/>
+        <v>23.953872238110105</v>
+      </c>
+    </row>
+    <row r="26" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="G26" s="3">
+        <v>47.79</v>
+      </c>
+      <c r="H26" s="5">
+        <v>18.7</v>
+      </c>
+      <c r="I26" s="5"/>
+      <c r="K26" s="22">
+        <f t="shared" si="7"/>
+        <v>9.35</v>
+      </c>
+      <c r="L26" s="20">
+        <f t="shared" si="8"/>
+        <v>3.735999999999999E-2</v>
+      </c>
+      <c r="M26" s="20">
+        <f t="shared" si="1"/>
+        <v>7.8049999999999994E-2</v>
+      </c>
+      <c r="N26" s="20">
+        <f t="shared" si="9"/>
+        <v>0.11757999999999999</v>
+      </c>
+      <c r="O26" s="20">
+        <f t="shared" si="10"/>
+        <v>0.15826999999999999</v>
+      </c>
+      <c r="P26" s="21">
+        <f t="shared" si="11"/>
+        <v>11.767764518443066</v>
+      </c>
+      <c r="Q26" s="21">
+        <f t="shared" si="5"/>
+        <v>0.82070607848243426</v>
+      </c>
+      <c r="R26" s="21">
+        <f t="shared" si="12"/>
+        <v>19.526197500884948</v>
+      </c>
+    </row>
+    <row r="28" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B28" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C28" s="15">
+        <f>C11*D11*D24*C23</f>
+        <v>222107.91366906479</v>
+      </c>
+      <c r="D28" s="15"/>
+    </row>
+    <row r="29" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B29" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C29" s="16">
+        <v>3.14E-10</v>
+      </c>
+      <c r="D29" s="17"/>
+    </row>
+    <row r="31" spans="2:18" x14ac:dyDescent="0.2">
+      <c r="B31" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C31" s="16">
+        <f>C28*C21/(2*PI())</f>
+        <v>4.4421582733812963E-2</v>
+      </c>
+      <c r="D31" s="17"/>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
+        <v>53</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="C23:D23"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
+  </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="45" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:P31"/>
   <sheetViews>

</xml_diff>